<commit_message>
Añadidos tests para informes y functions.py
</commit_message>
<xml_diff>
--- a/analysis/plantilla_informes.xlsx
+++ b/analysis/plantilla_informes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Nextcloud\Programacion\GitHub\contabilidad\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF5EDC4-745F-4ADD-98BB-25026C7BE25D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E74A4D6-0BE9-48A2-97D4-ADFAB5732EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="7800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="3" r:id="rId1"/>
     <sheet name="compleja" sheetId="2" r:id="rId2"/>
-    <sheet name="Cuentas" sheetId="4" r:id="rId3"/>
+    <sheet name="cuentas" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,15 +34,25 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
@@ -54,11 +62,16 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="135">
   <si>
     <t>Fecha</t>
   </si>
@@ -444,12 +457,6 @@
     <t>balance</t>
   </si>
   <si>
-    <t>gasto</t>
-  </si>
-  <si>
-    <t>ingreso</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -460,6 +467,15 @@
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>gastos, casa</t>
+  </si>
+  <si>
+    <t>gastos</t>
+  </si>
+  <si>
+    <t>ingresos</t>
   </si>
 </sst>
 </file>
@@ -2407,6 +2423,65 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <fb t="e">#NAME?</fb>
+    <v>4</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{778F37C6-8B26-4AC1-8C4D-65D6FCB16381}" name="Mov_simple" displayName="Mov_simple" ref="B3:H242" totalsRowShown="0">
   <autoFilter ref="B3:H242" xr:uid="{47D0FA3E-EDD9-4A2A-92E8-A35A238EDB76}"/>
@@ -2766,24 +2841,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C68A8C-4B2B-40F9-A6AA-47048CD7600B}">
   <dimension ref="B3:N242"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="8" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2810,10 +2885,10 @@
       </c>
       <c r="N3" s="17">
         <f ca="1">ROUND(10+RAND()*10, 2)</f>
-        <v>17.010000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+        <v>14.78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>44562</v>
       </c>
@@ -2838,7 +2913,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <v>44563</v>
       </c>
@@ -2869,10 +2944,10 @@
         <v>1</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>44564</v>
       </c>
@@ -2896,18 +2971,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Gastos coche</v>
       </c>
-      <c r="J6" t="str" cm="1">
-        <f t="array" ref="J6:L49">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(K3,Cuentas[Descripción]))))</f>
-        <v>100</v>
-      </c>
-      <c r="K6" t="str">
-        <v>Caja</v>
-      </c>
-      <c r="L6" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J6" t="e" cm="1" vm="1">
+        <f t="array" ref="J6:L49" ca="1">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(K3,Cuentas[Descripción]))))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>44570</v>
       </c>
@@ -2931,17 +3008,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Ropa</v>
       </c>
-      <c r="J7" t="str">
-        <v>101</v>
-      </c>
-      <c r="K7" t="str">
-        <v>Tickets restaurant</v>
-      </c>
-      <c r="L7" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="28">
         <v>44572</v>
       </c>
@@ -2965,17 +3045,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J8" t="str">
-        <v>1101</v>
-      </c>
-      <c r="K8" t="str">
-        <v>Cuenta nómina</v>
-      </c>
-      <c r="L8" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J8" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K8" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L8" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>44573</v>
       </c>
@@ -2999,17 +3082,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J9" t="str">
-        <v>1110</v>
-      </c>
-      <c r="K9" t="str">
-        <v>Cuenta ahorro</v>
-      </c>
-      <c r="L9" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J9" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K9" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L9" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="18">
         <v>44575</v>
       </c>
@@ -3033,17 +3119,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J10" t="str">
-        <v>1200</v>
-      </c>
-      <c r="K10" t="str">
-        <v>Tarjeta Visa</v>
-      </c>
-      <c r="L10" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J10" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K10" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L10" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>44576</v>
       </c>
@@ -3067,17 +3156,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Médicos</v>
       </c>
-      <c r="J11" t="str">
-        <v>1201</v>
-      </c>
-      <c r="K11" t="str">
-        <v>Tarjeta Amex</v>
-      </c>
-      <c r="L11" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J11" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K11" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L11" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
         <v>44577</v>
       </c>
@@ -3101,17 +3193,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J12" t="str">
-        <v>1210</v>
-      </c>
-      <c r="K12" t="str">
-        <v>Tarjeta prepago</v>
-      </c>
-      <c r="L12" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J12" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K12" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L12" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="28">
         <v>44578</v>
       </c>
@@ -3135,17 +3230,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Deportes</v>
       </c>
-      <c r="J13" t="str">
-        <v>1300</v>
-      </c>
-      <c r="K13" t="str">
-        <v>Paypal</v>
-      </c>
-      <c r="L13" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J13" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K13" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L13" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
         <v>44579</v>
       </c>
@@ -3169,17 +3267,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Refrescos, pinchos, etc</v>
       </c>
-      <c r="J14" t="str">
-        <v>1400</v>
-      </c>
-      <c r="K14" t="str">
-        <v>Fondo inversión</v>
-      </c>
-      <c r="L14" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J14" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K14" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L14" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>44579</v>
       </c>
@@ -3203,17 +3304,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Caja</v>
       </c>
-      <c r="J15" t="str">
-        <v>1401</v>
-      </c>
-      <c r="K15" t="str">
-        <v>Plan pensiones</v>
-      </c>
-      <c r="L15" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J15" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K15" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L15" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>44580</v>
       </c>
@@ -3237,17 +3341,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Donaciones</v>
       </c>
-      <c r="J16" t="str">
-        <v>150</v>
-      </c>
-      <c r="K16" t="str">
-        <v>Hipoteca</v>
-      </c>
-      <c r="L16" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J16" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K16" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L16" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>44581</v>
       </c>
@@ -3271,17 +3378,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Médicos</v>
       </c>
-      <c r="J17" t="str">
-        <v>151</v>
-      </c>
-      <c r="K17" t="str">
-        <v>Comisiones, intereses</v>
-      </c>
-      <c r="L17" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J17" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K17" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L17" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="18">
         <v>44582</v>
       </c>
@@ -3305,17 +3415,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J18" t="str">
-        <v>2000</v>
-      </c>
-      <c r="K18" t="str">
-        <v>Electricidad casa</v>
-      </c>
-      <c r="L18" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J18" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K18" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L18" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>44584</v>
       </c>
@@ -3339,17 +3452,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J19" t="str">
-        <v>2001</v>
-      </c>
-      <c r="K19" t="str">
-        <v>Gas casa</v>
-      </c>
-      <c r="L19" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J19" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K19" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L19" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>44584</v>
       </c>
@@ -3373,17 +3489,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>IT / Electrónica</v>
       </c>
-      <c r="J20" t="str">
-        <v>2002</v>
-      </c>
-      <c r="K20" t="str">
-        <v>Agua casa</v>
-      </c>
-      <c r="L20" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J20" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K20" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L20" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
         <v>44586</v>
       </c>
@@ -3407,17 +3526,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Gastos coche</v>
       </c>
-      <c r="J21" t="str">
-        <v>2003</v>
-      </c>
-      <c r="K21" t="str">
-        <v>Teléfono e internet casa</v>
-      </c>
-      <c r="L21" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J21" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K21" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L21" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>44586</v>
       </c>
@@ -3441,17 +3563,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Cuenta nómina</v>
       </c>
-      <c r="J22" t="str">
-        <v>2004</v>
-      </c>
-      <c r="K22" t="str">
-        <v>Seguro casa</v>
-      </c>
-      <c r="L22" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J22" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K22" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L22" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="13">
         <v>44589</v>
       </c>
@@ -3475,17 +3600,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J23" t="str">
-        <v>2005</v>
-      </c>
-      <c r="K23" t="str">
-        <v>Alarma casa</v>
-      </c>
-      <c r="L23" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J23" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K23" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L23" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19">
         <v>44591</v>
       </c>
@@ -3509,17 +3637,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J24" t="str">
-        <v>2006</v>
-      </c>
-      <c r="K24" t="str">
-        <v>Comunidad casa</v>
-      </c>
-      <c r="L24" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J24" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K24" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L24" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="19">
         <v>44592</v>
       </c>
@@ -3543,17 +3674,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Tarjeta Visa</v>
       </c>
-      <c r="J25" t="str">
-        <v>2007</v>
-      </c>
-      <c r="K25" t="str">
-        <v>Limpieza casa</v>
-      </c>
-      <c r="L25" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J25" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K25" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L25" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="19">
         <v>44593</v>
       </c>
@@ -3577,17 +3711,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Caja</v>
       </c>
-      <c r="J26" t="str">
-        <v>201</v>
-      </c>
-      <c r="K26" t="str">
-        <v>Muebles, electrodomésticos casa</v>
-      </c>
-      <c r="L26" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J26" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K26" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L26" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="19">
         <v>44594</v>
       </c>
@@ -3611,17 +3748,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Refrescos, pinchos, etc</v>
       </c>
-      <c r="J27" t="str">
-        <v>202</v>
-      </c>
-      <c r="K27" t="str">
-        <v>Obras, reformas casa</v>
-      </c>
-      <c r="L27" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J27" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K27" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L27" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>44596</v>
       </c>
@@ -3645,17 +3785,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J28" t="str">
-        <v>203</v>
-      </c>
-      <c r="K28" t="str">
-        <v>Impuestos casa</v>
-      </c>
-      <c r="L28" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J28" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K28" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L28" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="19">
         <v>44598</v>
       </c>
@@ -3679,17 +3822,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J29" t="str">
-        <v>204</v>
-      </c>
-      <c r="K29" t="str">
-        <v>Jardín casa</v>
-      </c>
-      <c r="L29" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J29" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K29" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L29" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="13">
         <v>44603</v>
       </c>
@@ -3713,17 +3859,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J30" t="str">
-        <v>205</v>
-      </c>
-      <c r="K30" t="str">
-        <v>Gastos varios casa</v>
-      </c>
-      <c r="L30" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J30" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K30" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L30" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="19">
         <v>44604</v>
       </c>
@@ -3747,17 +3896,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J31" t="str">
-        <v>300</v>
-      </c>
-      <c r="K31" t="str">
-        <v>Comida</v>
-      </c>
-      <c r="L31" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J31" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K31" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L31" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="19">
         <v>44605</v>
       </c>
@@ -3781,17 +3933,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J32" t="str">
-        <v>301</v>
-      </c>
-      <c r="K32" t="str">
-        <v>Ropa</v>
-      </c>
-      <c r="L32" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J32" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K32" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L32" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="13">
         <v>44608</v>
       </c>
@@ -3815,17 +3970,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Gastos coche</v>
       </c>
-      <c r="J33" t="str">
-        <v>302</v>
-      </c>
-      <c r="K33" t="str">
-        <v>Higiene personal</v>
-      </c>
-      <c r="L33" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J33" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K33" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L33" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="19">
         <v>44610</v>
       </c>
@@ -3849,17 +4007,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Refrescos, pinchos, etc</v>
       </c>
-      <c r="J34" t="str">
-        <v>310</v>
-      </c>
-      <c r="K34" t="str">
-        <v>Refrescos, pinchos, etc</v>
-      </c>
-      <c r="L34" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J34" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K34" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L34" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="13">
         <v>44610</v>
       </c>
@@ -3883,17 +4044,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J35" t="str">
-        <v>311</v>
-      </c>
-      <c r="K35" t="str">
-        <v>Cine, teatro, conciertos…</v>
-      </c>
-      <c r="L35" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J35" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K35" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L35" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="19">
         <v>44610</v>
       </c>
@@ -3917,17 +4081,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Caja</v>
       </c>
-      <c r="J36" t="str">
-        <v>312</v>
-      </c>
-      <c r="K36" t="str">
-        <v>Comidas, cenas…</v>
-      </c>
-      <c r="L36" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J36" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K36" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L36" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="19">
         <v>44610</v>
       </c>
@@ -3951,17 +4118,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>IT / Electrónica</v>
       </c>
-      <c r="J37" t="str">
-        <v>320</v>
-      </c>
-      <c r="K37" t="str">
-        <v>Vacaciones - Salidas</v>
-      </c>
-      <c r="L37" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J37" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K37" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L37" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="19">
         <v>44611</v>
       </c>
@@ -3985,17 +4155,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Donaciones</v>
       </c>
-      <c r="J38" t="str">
-        <v>324</v>
-      </c>
-      <c r="K38" t="str">
-        <v>Gastos coche</v>
-      </c>
-      <c r="L38" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J38" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K38" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L38" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="19">
         <v>44612</v>
       </c>
@@ -4019,17 +4192,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J39" t="str">
-        <v>33</v>
-      </c>
-      <c r="K39" t="str">
-        <v>Médicos</v>
-      </c>
-      <c r="L39" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J39" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K39" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L39" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="19">
         <v>44617</v>
       </c>
@@ -4053,17 +4229,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Cuenta nómina</v>
       </c>
-      <c r="J40" t="str">
-        <v>340</v>
-      </c>
-      <c r="K40" t="str">
-        <v>Deportes</v>
-      </c>
-      <c r="L40" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J40" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K40" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L40" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="13">
         <v>44617</v>
       </c>
@@ -4087,17 +4266,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J41" t="str">
-        <v>343</v>
-      </c>
-      <c r="K41" t="str">
-        <v>IT / Electrónica</v>
-      </c>
-      <c r="L41" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J41" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K41" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L41" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="19">
         <v>44619</v>
       </c>
@@ -4121,17 +4303,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J42" t="str">
-        <v>35</v>
-      </c>
-      <c r="K42" t="str">
-        <v>Educación, cultura</v>
-      </c>
-      <c r="L42" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J42" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K42" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L42" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="19">
         <v>44620</v>
       </c>
@@ -4155,17 +4340,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Tarjeta Visa</v>
       </c>
-      <c r="J43" t="str">
-        <v>36</v>
-      </c>
-      <c r="K43" t="str">
-        <v>Impuestos</v>
-      </c>
-      <c r="L43" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J43" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K43" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L43" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="19">
         <v>44621</v>
       </c>
@@ -4189,17 +4377,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Caja</v>
       </c>
-      <c r="J44" t="str">
-        <v>370</v>
-      </c>
-      <c r="K44" t="str">
-        <v>Donaciones</v>
-      </c>
-      <c r="L44" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J44" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K44" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L44" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <v>44624</v>
       </c>
@@ -4223,17 +4414,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J45" t="str">
-        <v>374</v>
-      </c>
-      <c r="K45" t="str">
-        <v>Otros gastos</v>
-      </c>
-      <c r="L45" t="str">
-        <v>gasto</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J45" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K45" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L45" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="19">
         <v>44626</v>
       </c>
@@ -4257,17 +4451,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Refrescos, pinchos, etc</v>
       </c>
-      <c r="J46" t="str">
-        <v>400</v>
-      </c>
-      <c r="K46" t="str">
-        <v>Nómina</v>
-      </c>
-      <c r="L46" t="str">
-        <v>ingreso</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J46" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K46" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L46" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="19">
         <v>44626</v>
       </c>
@@ -4291,17 +4488,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comida</v>
       </c>
-      <c r="J47" t="str">
-        <v>410</v>
-      </c>
-      <c r="K47" t="str">
-        <v>Intereses bancos</v>
-      </c>
-      <c r="L47" t="str">
-        <v>ingreso</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J47" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K47" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L47" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="19">
         <v>44630</v>
       </c>
@@ -4325,17 +4525,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Gastos coche</v>
       </c>
-      <c r="J48" t="str">
-        <v>43</v>
-      </c>
-      <c r="K48" t="str">
-        <v>Otros ingresos</v>
-      </c>
-      <c r="L48" t="str">
-        <v>ingreso</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J48" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K48" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L48" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="13">
         <v>44631</v>
       </c>
@@ -4359,17 +4562,20 @@
         <f>VLOOKUP(Mov_simple[[#This Row],[Haber]],Cuentas[],2,FALSE)</f>
         <v>Comidas, cenas…</v>
       </c>
-      <c r="J49" t="str">
-        <v>60</v>
-      </c>
-      <c r="K49" t="str">
-        <v>Ajustes</v>
-      </c>
-      <c r="L49" t="str">
-        <v>balance</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J49" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K49" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L49" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="19">
         <v>44633</v>
       </c>
@@ -4394,7 +4600,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="19">
         <v>44635</v>
       </c>
@@ -4419,7 +4625,7 @@
         <v>Ropa</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="19">
         <v>44636</v>
       </c>
@@ -4444,7 +4650,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="19">
         <v>44636</v>
       </c>
@@ -4469,7 +4675,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="13">
         <v>44638</v>
       </c>
@@ -4494,7 +4700,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="19">
         <v>44638</v>
       </c>
@@ -4519,7 +4725,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="19">
         <v>44639</v>
       </c>
@@ -4544,7 +4750,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="19">
         <v>44640</v>
       </c>
@@ -4569,7 +4775,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="19">
         <v>44642</v>
       </c>
@@ -4594,7 +4800,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="19">
         <v>44643</v>
       </c>
@@ -4619,7 +4825,7 @@
         <v>Médicos</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="19">
         <v>44645</v>
       </c>
@@ -4644,7 +4850,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="13">
         <v>44645</v>
       </c>
@@ -4669,7 +4875,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="19">
         <v>44647</v>
       </c>
@@ -4694,7 +4900,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="19">
         <v>44651</v>
       </c>
@@ -4719,7 +4925,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="13">
         <v>44652</v>
       </c>
@@ -4744,7 +4950,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="13">
         <v>44652</v>
       </c>
@@ -4769,7 +4975,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="19">
         <v>44652</v>
       </c>
@@ -4794,7 +5000,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="19">
         <v>44654</v>
       </c>
@@ -4819,7 +5025,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="19">
         <v>44658</v>
       </c>
@@ -4844,7 +5050,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="13">
         <v>44659</v>
       </c>
@@ -4869,7 +5075,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="19">
         <v>44661</v>
       </c>
@@ -4894,7 +5100,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="19">
         <v>44662</v>
       </c>
@@ -4919,7 +5125,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="13">
         <v>44666</v>
       </c>
@@ -4944,7 +5150,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="19">
         <v>44668</v>
       </c>
@@ -4969,7 +5175,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="19">
         <v>44668</v>
       </c>
@@ -4994,7 +5200,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="28">
         <v>44669</v>
       </c>
@@ -5019,7 +5225,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
         <v>44670</v>
       </c>
@@ -5044,7 +5250,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="18">
         <v>44673</v>
       </c>
@@ -5069,7 +5275,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="28">
         <v>44674</v>
       </c>
@@ -5094,7 +5300,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="28">
         <v>44674</v>
       </c>
@@ -5119,7 +5325,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="28">
         <v>44675</v>
       </c>
@@ -5144,7 +5350,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="28">
         <v>44676</v>
       </c>
@@ -5169,7 +5375,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="18">
         <v>44680</v>
       </c>
@@ -5194,7 +5400,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="28">
         <v>44681</v>
       </c>
@@ -5219,7 +5425,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="28">
         <v>44682</v>
       </c>
@@ -5244,7 +5450,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>44682</v>
       </c>
@@ -5269,7 +5475,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="18">
         <v>44687</v>
       </c>
@@ -5294,7 +5500,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
         <v>44688</v>
       </c>
@@ -5319,7 +5525,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="28">
         <v>44689</v>
       </c>
@@ -5344,7 +5550,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="28">
         <v>44690</v>
       </c>
@@ -5369,7 +5575,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="18">
         <v>44694</v>
       </c>
@@ -5394,7 +5600,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="28">
         <v>44696</v>
       </c>
@@ -5419,7 +5625,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="18">
         <v>44696</v>
       </c>
@@ -5444,7 +5650,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="28">
         <v>44699</v>
       </c>
@@ -5469,7 +5675,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>44700</v>
       </c>
@@ -5494,7 +5700,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>44700</v>
       </c>
@@ -5519,7 +5725,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="18">
         <v>44701</v>
       </c>
@@ -5544,7 +5750,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="28">
         <v>44703</v>
       </c>
@@ -5569,7 +5775,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="28">
         <v>44706</v>
       </c>
@@ -5594,7 +5800,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="28">
         <v>44706</v>
       </c>
@@ -5619,7 +5825,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="18">
         <v>44708</v>
       </c>
@@ -5644,7 +5850,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="28">
         <v>44710</v>
       </c>
@@ -5669,7 +5875,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="28">
         <v>44710</v>
       </c>
@@ -5694,7 +5900,7 @@
         <v>Médicos</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
         <v>44712</v>
       </c>
@@ -5719,7 +5925,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="1">
         <v>44713</v>
       </c>
@@ -5744,7 +5950,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="20">
         <v>44714</v>
       </c>
@@ -5769,7 +5975,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="18">
         <v>44715</v>
       </c>
@@ -5794,7 +6000,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="20">
         <v>44717</v>
       </c>
@@ -5819,7 +6025,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="1">
         <v>44717</v>
       </c>
@@ -5844,7 +6050,7 @@
         <v>Impuestos casa</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="20">
         <v>44718</v>
       </c>
@@ -5869,7 +6075,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="28">
         <v>44722</v>
       </c>
@@ -5894,7 +6100,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="12">
         <v>44722</v>
       </c>
@@ -5919,7 +6125,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="28">
         <v>44724</v>
       </c>
@@ -5944,7 +6150,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="12">
         <v>44729</v>
       </c>
@@ -5969,7 +6175,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="1">
         <v>44730</v>
       </c>
@@ -5994,7 +6200,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" s="20">
         <v>44731</v>
       </c>
@@ -6019,7 +6225,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" s="1">
         <v>44731</v>
       </c>
@@ -6044,7 +6250,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" s="20">
         <v>44732</v>
       </c>
@@ -6069,7 +6275,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="18">
         <v>44736</v>
       </c>
@@ -6094,7 +6300,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="20">
         <v>44737</v>
       </c>
@@ -6119,7 +6325,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="28">
         <v>44738</v>
       </c>
@@ -6144,7 +6350,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="20">
         <v>44738</v>
       </c>
@@ -6169,7 +6375,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="18">
         <v>44740</v>
       </c>
@@ -6194,7 +6400,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
         <v>44740</v>
       </c>
@@ -6219,7 +6425,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="1">
         <v>44742</v>
       </c>
@@ -6244,7 +6450,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="18">
         <v>44743</v>
       </c>
@@ -6269,7 +6475,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="1">
         <v>44743</v>
       </c>
@@ -6294,7 +6500,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="28">
         <v>44745</v>
       </c>
@@ -6319,7 +6525,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" s="18">
         <v>44750</v>
       </c>
@@ -6344,7 +6550,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="28">
         <v>44752</v>
       </c>
@@ -6369,7 +6575,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="28">
         <v>44754</v>
       </c>
@@ -6394,7 +6600,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="18">
         <v>44757</v>
       </c>
@@ -6419,7 +6625,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="28">
         <v>44759</v>
       </c>
@@ -6444,7 +6650,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="1">
         <v>44760</v>
       </c>
@@ -6469,7 +6675,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="1">
         <v>44761</v>
       </c>
@@ -6494,7 +6700,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="28">
         <v>44762</v>
       </c>
@@ -6519,7 +6725,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" s="28">
         <v>44764</v>
       </c>
@@ -6544,7 +6750,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" s="18">
         <v>44764</v>
       </c>
@@ -6569,7 +6775,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="28">
         <v>44766</v>
       </c>
@@ -6594,7 +6800,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="1">
         <v>44766</v>
       </c>
@@ -6619,7 +6825,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" s="28">
         <v>44767</v>
       </c>
@@ -6644,7 +6850,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="28">
         <v>44770</v>
       </c>
@@ -6669,7 +6875,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="18">
         <v>44771</v>
       </c>
@@ -6694,7 +6900,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" s="1">
         <v>44773</v>
       </c>
@@ -6719,7 +6925,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" s="28">
         <v>44773</v>
       </c>
@@ -6744,7 +6950,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" s="1">
         <v>44774</v>
       </c>
@@ -6769,7 +6975,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" s="1">
         <v>44777</v>
       </c>
@@ -6794,7 +7000,7 @@
         <v>Médicos</v>
       </c>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" s="18">
         <v>44778</v>
       </c>
@@ -6819,7 +7025,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" s="28">
         <v>44780</v>
       </c>
@@ -6844,7 +7050,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" s="18">
         <v>44784</v>
       </c>
@@ -6869,7 +7075,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" s="18">
         <v>44785</v>
       </c>
@@ -6894,7 +7100,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" s="28">
         <v>44786</v>
       </c>
@@ -6919,7 +7125,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" s="28">
         <v>44787</v>
       </c>
@@ -6944,7 +7150,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" s="1">
         <v>44791</v>
       </c>
@@ -6969,7 +7175,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" s="18">
         <v>44792</v>
       </c>
@@ -6994,7 +7200,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" s="1">
         <v>44792</v>
       </c>
@@ -7019,7 +7225,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B156" s="1">
         <v>44792</v>
       </c>
@@ -7044,7 +7250,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" s="28">
         <v>44794</v>
       </c>
@@ -7069,7 +7275,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" s="28">
         <v>44796</v>
       </c>
@@ -7094,7 +7300,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" s="28">
         <v>44798</v>
       </c>
@@ -7119,7 +7325,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B160" s="18">
         <v>44799</v>
       </c>
@@ -7144,7 +7350,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B161" s="28">
         <v>44801</v>
       </c>
@@ -7169,7 +7375,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B162" s="28">
         <v>44802</v>
       </c>
@@ -7194,7 +7400,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B163" s="1">
         <v>44804</v>
       </c>
@@ -7219,7 +7425,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B164" s="1">
         <v>44805</v>
       </c>
@@ -7244,7 +7450,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" s="1">
         <v>44806</v>
       </c>
@@ -7269,7 +7475,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" s="18">
         <v>44806</v>
       </c>
@@ -7294,7 +7500,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" s="28">
         <v>44808</v>
       </c>
@@ -7319,7 +7525,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="168" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B168" s="18">
         <v>44813</v>
       </c>
@@ -7344,7 +7550,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" s="28">
         <v>44815</v>
       </c>
@@ -7369,7 +7575,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" s="28">
         <v>44818</v>
       </c>
@@ -7394,7 +7600,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" s="1">
         <v>44818</v>
       </c>
@@ -7419,7 +7625,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" s="18">
         <v>44820</v>
       </c>
@@ -7444,7 +7650,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="173" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B173" s="28">
         <v>44822</v>
       </c>
@@ -7469,7 +7675,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="174" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B174" s="1">
         <v>44822</v>
       </c>
@@ -7494,7 +7700,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B175" s="1">
         <v>44823</v>
       </c>
@@ -7519,7 +7725,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" s="18">
         <v>44827</v>
       </c>
@@ -7544,7 +7750,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" s="28">
         <v>44828</v>
       </c>
@@ -7569,7 +7775,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" s="18">
         <v>44828</v>
       </c>
@@ -7594,7 +7800,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B179" s="28">
         <v>44829</v>
       </c>
@@ -7619,7 +7825,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" s="1">
         <v>44829</v>
       </c>
@@ -7644,7 +7850,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B181" s="1">
         <v>44834</v>
       </c>
@@ -7669,7 +7875,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B182" s="28">
         <v>44834</v>
       </c>
@@ -7694,7 +7900,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" s="18">
         <v>44834</v>
       </c>
@@ -7719,7 +7925,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" s="1">
         <v>44835</v>
       </c>
@@ -7744,7 +7950,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" s="28">
         <v>44836</v>
       </c>
@@ -7769,7 +7975,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B186" s="18">
         <v>44841</v>
       </c>
@@ -7794,7 +8000,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B187" s="28">
         <v>44843</v>
       </c>
@@ -7819,7 +8025,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B188" s="1">
         <v>44844</v>
       </c>
@@ -7844,7 +8050,7 @@
         <v>Médicos</v>
       </c>
     </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" s="1">
         <v>44844</v>
       </c>
@@ -7869,7 +8075,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B190" s="18">
         <v>44848</v>
       </c>
@@ -7894,7 +8100,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="191" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B191" s="28">
         <v>44850</v>
       </c>
@@ -7919,7 +8125,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="192" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B192" s="28">
         <v>44850</v>
       </c>
@@ -7944,7 +8150,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="193" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B193" s="1">
         <v>44850</v>
       </c>
@@ -7969,7 +8175,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B194" s="1">
         <v>44852</v>
       </c>
@@ -7994,7 +8200,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="195" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B195" s="1">
         <v>44853</v>
       </c>
@@ -8019,7 +8225,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="196" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B196" s="18">
         <v>44855</v>
       </c>
@@ -8044,7 +8250,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="197" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B197" s="28">
         <v>44857</v>
       </c>
@@ -8069,7 +8275,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B198" s="1">
         <v>44859</v>
       </c>
@@ -8094,7 +8300,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B199" s="28">
         <v>44860</v>
       </c>
@@ -8119,7 +8325,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B200" s="18">
         <v>44862</v>
       </c>
@@ -8144,7 +8350,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="201" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B201" s="28">
         <v>44864</v>
       </c>
@@ -8169,7 +8375,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="202" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B202" s="1">
         <v>44865</v>
       </c>
@@ -8194,7 +8400,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="203" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B203" s="28">
         <v>44866</v>
       </c>
@@ -8219,7 +8425,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B204" s="1">
         <v>44866</v>
       </c>
@@ -8244,7 +8450,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="205" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B205" s="18">
         <v>44869</v>
       </c>
@@ -8269,7 +8475,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B206" s="1">
         <v>44870</v>
       </c>
@@ -8294,7 +8500,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B207" s="28">
         <v>44871</v>
       </c>
@@ -8319,7 +8525,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B208" s="18">
         <v>44872</v>
       </c>
@@ -8344,7 +8550,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="209" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B209" s="18">
         <v>44876</v>
       </c>
@@ -8369,7 +8575,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="210" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B210" s="28">
         <v>44878</v>
       </c>
@@ -8394,7 +8600,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="211" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" s="28">
         <v>44882</v>
       </c>
@@ -8419,7 +8625,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="212" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B212" s="18">
         <v>44883</v>
       </c>
@@ -8444,7 +8650,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="213" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B213" s="1">
         <v>44883</v>
       </c>
@@ -8469,7 +8675,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="214" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B214" s="1">
         <v>44884</v>
       </c>
@@ -8494,7 +8700,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="215" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B215" s="28">
         <v>44885</v>
       </c>
@@ -8519,7 +8725,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="216" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B216" s="1">
         <v>44890</v>
       </c>
@@ -8544,7 +8750,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="217" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B217" s="18">
         <v>44890</v>
       </c>
@@ -8569,7 +8775,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="218" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B218" s="28">
         <v>44892</v>
       </c>
@@ -8594,7 +8800,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="219" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B219" s="28">
         <v>44892</v>
       </c>
@@ -8619,7 +8825,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="220" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B220" s="1">
         <v>44894</v>
       </c>
@@ -8644,7 +8850,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="221" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B221" s="1">
         <v>44895</v>
       </c>
@@ -8669,7 +8875,7 @@
         <v>Tarjeta Visa</v>
       </c>
     </row>
-    <row r="222" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B222" s="1">
         <v>44896</v>
       </c>
@@ -8694,7 +8900,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="223" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B223" s="1">
         <v>44896</v>
       </c>
@@ -8719,7 +8925,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="224" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B224" s="18">
         <v>44897</v>
       </c>
@@ -8744,7 +8950,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="225" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B225" s="28">
         <v>44898</v>
       </c>
@@ -8769,7 +8975,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="226" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B226" s="28">
         <v>44899</v>
       </c>
@@ -8794,7 +9000,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="227" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B227" s="18">
         <v>44904</v>
       </c>
@@ -8819,7 +9025,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="228" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B228" s="28">
         <v>44906</v>
       </c>
@@ -8844,7 +9050,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="229" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B229" s="1">
         <v>44911</v>
       </c>
@@ -8869,7 +9075,7 @@
         <v>Médicos</v>
       </c>
     </row>
-    <row r="230" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B230" s="18">
         <v>44911</v>
       </c>
@@ -8894,7 +9100,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="231" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B231" s="28">
         <v>44913</v>
       </c>
@@ -8919,7 +9125,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="232" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B232" s="1">
         <v>44913</v>
       </c>
@@ -8944,7 +9150,7 @@
         <v>Caja</v>
       </c>
     </row>
-    <row r="233" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B233" s="28">
         <v>44914</v>
       </c>
@@ -8969,7 +9175,7 @@
         <v>Refrescos, pinchos, etc</v>
       </c>
     </row>
-    <row r="234" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B234" s="1">
         <v>44914</v>
       </c>
@@ -8994,7 +9200,7 @@
         <v>Donaciones</v>
       </c>
     </row>
-    <row r="235" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B235" s="18">
         <v>44916</v>
       </c>
@@ -9019,7 +9225,7 @@
         <v>Gastos coche</v>
       </c>
     </row>
-    <row r="236" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B236" s="18">
         <v>44918</v>
       </c>
@@ -9044,7 +9250,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="237" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B237" s="28">
         <v>44920</v>
       </c>
@@ -9069,7 +9275,7 @@
         <v>Comida</v>
       </c>
     </row>
-    <row r="238" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B238" s="28">
         <v>44920</v>
       </c>
@@ -9094,7 +9300,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="239" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B239" s="1">
         <v>44922</v>
       </c>
@@ -9119,7 +9325,7 @@
         <v>IT / Electrónica</v>
       </c>
     </row>
-    <row r="240" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B240" s="28">
         <v>44924</v>
       </c>
@@ -9144,7 +9350,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="241" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" s="18">
         <v>44925</v>
       </c>
@@ -9169,7 +9375,7 @@
         <v>Comidas, cenas…</v>
       </c>
     </row>
-    <row r="242" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" s="1">
         <v>44926</v>
       </c>
@@ -9212,21 +9418,21 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" customWidth="1"/>
-    <col min="5" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.44140625" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -9267,7 +9473,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -9304,7 +9510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -9347,7 +9553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -9383,18 +9589,20 @@
       <c r="M6" s="6">
         <v>0</v>
       </c>
-      <c r="O6" t="str" cm="1">
-        <f t="array" ref="O6:Q6">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
-        <v>410</v>
-      </c>
-      <c r="P6" t="str">
-        <v>Intereses bancos</v>
-      </c>
-      <c r="Q6" t="str">
-        <v>ingreso</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O6" t="e" cm="1" vm="1">
+        <f t="array" ref="O6:Q6" ca="1">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -9431,7 +9639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
@@ -9449,7 +9657,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H8" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -9468,7 +9676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
@@ -9506,7 +9714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
@@ -9543,7 +9751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -9580,7 +9788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2</v>
       </c>
@@ -9617,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3</v>
       </c>
@@ -9654,7 +9862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3</v>
       </c>
@@ -9691,7 +9899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
@@ -9728,7 +9936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>4</v>
       </c>
@@ -9765,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>4</v>
       </c>
@@ -9784,7 +9992,7 @@
         <v>416.66666666666669</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H17" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -9803,7 +10011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>4</v>
       </c>
@@ -9822,7 +10030,7 @@
         <v>583.33333333333326</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H18" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -9841,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>5</v>
       </c>
@@ -9878,7 +10086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>5</v>
       </c>
@@ -9897,7 +10105,7 @@
         <v>412.5</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H20" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -9916,7 +10124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5</v>
       </c>
@@ -9935,7 +10143,7 @@
         <v>587.5</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H21" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -9954,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>6</v>
       </c>
@@ -9991,7 +10199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6</v>
       </c>
@@ -10010,7 +10218,7 @@
         <v>408.33333333333331</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H23" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -10029,7 +10237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>6</v>
       </c>
@@ -10048,7 +10256,7 @@
         <v>591.66666666666674</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H24" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
@@ -10067,7 +10275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>7</v>
       </c>
@@ -10092,7 +10300,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>7</v>
       </c>
@@ -10111,14 +10319,14 @@
         <v>404.16666666666669</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H26" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>7</v>
       </c>
@@ -10137,14 +10345,14 @@
         <v>595.83333333333326</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>8</v>
       </c>
@@ -10169,7 +10377,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>8</v>
       </c>
@@ -10188,14 +10396,14 @@
         <v>400</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H29" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>8</v>
       </c>
@@ -10214,14 +10422,14 @@
         <v>600</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H30" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>9</v>
       </c>
@@ -10246,7 +10454,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>9</v>
       </c>
@@ -10265,14 +10473,14 @@
         <v>395.83333333333331</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H32" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>9</v>
       </c>
@@ -10291,14 +10499,14 @@
         <v>604.16666666666674</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H33" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>10</v>
       </c>
@@ -10323,7 +10531,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>10</v>
       </c>
@@ -10342,14 +10550,14 @@
         <v>391.66666666666669</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H35" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>10</v>
       </c>
@@ -10368,14 +10576,14 @@
         <v>608.33333333333326</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H36" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>11</v>
       </c>
@@ -10400,7 +10608,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>11</v>
       </c>
@@ -10419,14 +10627,14 @@
         <v>387.5</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H38" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>11</v>
       </c>
@@ -10445,14 +10653,14 @@
         <v>612.5</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H39" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>12</v>
       </c>
@@ -10477,7 +10685,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>12</v>
       </c>
@@ -10496,14 +10704,14 @@
         <v>383.33333333333331</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H41" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>12</v>
       </c>
@@ -10522,14 +10730,14 @@
         <v>616.66666666666674</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H42" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>13</v>
       </c>
@@ -10554,7 +10762,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>13</v>
       </c>
@@ -10573,14 +10781,14 @@
         <v>379.16666666666669</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H44" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>13</v>
       </c>
@@ -10599,14 +10807,14 @@
         <v>620.83333333333326</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H45" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>14</v>
       </c>
@@ -10631,7 +10839,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>14</v>
       </c>
@@ -10650,14 +10858,14 @@
         <v>375</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H47" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>14</v>
       </c>
@@ -10676,14 +10884,14 @@
         <v>625</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H48" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>15</v>
       </c>
@@ -10708,7 +10916,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>15</v>
       </c>
@@ -10727,14 +10935,14 @@
         <v>370.83333333333331</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H50" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Comisiones, intereses</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>15</v>
       </c>
@@ -10753,14 +10961,14 @@
         <v>629.16666666666674</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H51" s="5" t="str">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Hipoteca</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>16</v>
       </c>
@@ -10785,7 +10993,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>16</v>
       </c>
@@ -10810,7 +11018,7 @@
         <v>Gas casa</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>16</v>
       </c>
@@ -10835,7 +11043,7 @@
         <v>Electricidad casa</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>17</v>
       </c>
@@ -10860,7 +11068,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>17</v>
       </c>
@@ -10885,7 +11093,7 @@
         <v>Gas casa</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>17</v>
       </c>
@@ -10910,7 +11118,7 @@
         <v>Electricidad casa</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>18</v>
       </c>
@@ -10935,7 +11143,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>18</v>
       </c>
@@ -10960,7 +11168,7 @@
         <v>Gas casa</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>18</v>
       </c>
@@ -10985,7 +11193,7 @@
         <v>Electricidad casa</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>19</v>
       </c>
@@ -11010,7 +11218,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>19</v>
       </c>
@@ -11035,7 +11243,7 @@
         <v>Gas casa</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>19</v>
       </c>
@@ -11060,7 +11268,7 @@
         <v>Electricidad casa</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>20</v>
       </c>
@@ -11085,7 +11293,7 @@
         <v>Cuenta nómina</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>20</v>
       </c>
@@ -11110,7 +11318,7 @@
         <v>Gas casa</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>20</v>
       </c>
@@ -11153,17 +11361,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77992459-7EBD-4FF8-A263-AD3B398FEA90}">
   <dimension ref="B2:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>75</v>
       </c>
@@ -11171,7 +11380,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -11191,16 +11400,18 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="str" cm="1">
-        <f t="array" ref="B5:D7">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(C2,Cuentas[Descripción]))))</f>
-        <v>1200</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Tarjeta Visa</v>
-      </c>
-      <c r="D5" t="str">
-        <v>balance</v>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="e" cm="1" vm="1">
+        <f t="array" ref="B5:D7" ca="1">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(C2,Cuentas[Descripción]))))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C5" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D5" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -11212,15 +11423,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="str">
-        <v>1201</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Tarjeta Amex</v>
-      </c>
-      <c r="D6" t="str">
-        <v>balance</v>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="C6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D6" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -11232,15 +11446,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="str">
-        <v>1210</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Tarjeta prepago</v>
-      </c>
-      <c r="D7" t="str">
-        <v>balance</v>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="C7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D7" t="e" vm="1">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -11252,7 +11469,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>15</v>
       </c>
@@ -11263,7 +11480,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>16</v>
       </c>
@@ -11274,7 +11491,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>17</v>
       </c>
@@ -11285,7 +11502,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>18</v>
       </c>
@@ -11296,7 +11513,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>19</v>
       </c>
@@ -11307,7 +11524,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>21</v>
       </c>
@@ -11318,7 +11535,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>22</v>
       </c>
@@ -11329,29 +11546,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F15" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G15" t="s">
         <v>99</v>
       </c>
       <c r="H15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F16" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>23</v>
       </c>
@@ -11359,10 +11576,10 @@
         <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>25</v>
       </c>
@@ -11370,10 +11587,10 @@
         <v>26</v>
       </c>
       <c r="H18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>27</v>
       </c>
@@ -11381,10 +11598,10 @@
         <v>28</v>
       </c>
       <c r="H19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>29</v>
       </c>
@@ -11392,10 +11609,10 @@
         <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>30</v>
       </c>
@@ -11403,10 +11620,10 @@
         <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>32</v>
       </c>
@@ -11414,10 +11631,10 @@
         <v>33</v>
       </c>
       <c r="H22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>34</v>
       </c>
@@ -11425,10 +11642,10 @@
         <v>35</v>
       </c>
       <c r="H23" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>36</v>
       </c>
@@ -11436,10 +11653,10 @@
         <v>37</v>
       </c>
       <c r="H24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>38</v>
       </c>
@@ -11447,10 +11664,10 @@
         <v>39</v>
       </c>
       <c r="H25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>40</v>
       </c>
@@ -11458,10 +11675,10 @@
         <v>41</v>
       </c>
       <c r="H26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>42</v>
       </c>
@@ -11469,10 +11686,10 @@
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>44</v>
       </c>
@@ -11480,10 +11697,10 @@
         <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>84</v>
       </c>
@@ -11491,10 +11708,10 @@
         <v>45</v>
       </c>
       <c r="H29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="6:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>46</v>
       </c>
@@ -11502,10 +11719,10 @@
         <v>47</v>
       </c>
       <c r="H30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>48</v>
       </c>
@@ -11513,10 +11730,10 @@
         <v>49</v>
       </c>
       <c r="H31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>50</v>
       </c>
@@ -11524,10 +11741,10 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>52</v>
       </c>
@@ -11535,10 +11752,10 @@
         <v>53</v>
       </c>
       <c r="H33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>10</v>
       </c>
@@ -11546,10 +11763,10 @@
         <v>54</v>
       </c>
       <c r="H34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>55</v>
       </c>
@@ -11557,10 +11774,10 @@
         <v>56</v>
       </c>
       <c r="H35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>57</v>
       </c>
@@ -11568,10 +11785,10 @@
         <v>58</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>59</v>
       </c>
@@ -11579,10 +11796,10 @@
         <v>60</v>
       </c>
       <c r="H37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>89</v>
       </c>
@@ -11590,10 +11807,10 @@
         <v>90</v>
       </c>
       <c r="H38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>61</v>
       </c>
@@ -11601,10 +11818,10 @@
         <v>62</v>
       </c>
       <c r="H39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>63</v>
       </c>
@@ -11612,10 +11829,10 @@
         <v>64</v>
       </c>
       <c r="H40" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>88</v>
       </c>
@@ -11623,10 +11840,10 @@
         <v>87</v>
       </c>
       <c r="H41" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>65</v>
       </c>
@@ -11634,10 +11851,10 @@
         <v>66</v>
       </c>
       <c r="H42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>85</v>
       </c>
@@ -11645,10 +11862,10 @@
         <v>79</v>
       </c>
       <c r="H43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>86</v>
       </c>
@@ -11656,10 +11873,10 @@
         <v>67</v>
       </c>
       <c r="H44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>68</v>
       </c>
@@ -11667,10 +11884,10 @@
         <v>100</v>
       </c>
       <c r="H45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>69</v>
       </c>
@@ -11678,10 +11895,10 @@
         <v>70</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>71</v>
       </c>
@@ -11689,10 +11906,10 @@
         <v>72</v>
       </c>
       <c r="H47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>73</v>
       </c>

</xml_diff>